<commit_message>
Fix Protocol Liquidation Fee calculation.
</commit_message>
<xml_diff>
--- a/contracts/red-bank/tests/files/Red Bank - Dynamic LB & CF test cases v1.1.xlsx
+++ b/contracts/red-bank/tests/files/Red Bank - Dynamic LB & CF test cases v1.1.xlsx
@@ -952,12 +952,12 @@
         <v>39</v>
       </c>
       <c r="C41" s="8">
-        <f>CEILING(FLOOR(C40*C27,1)*C5,1)</f>
-        <v>11</v>
+        <f>FLOOR(CEILING(FLOOR(D38*C27,1)*C5,1)/D13,1)</f>
+        <v>9</v>
       </c>
       <c r="D41" s="8">
         <f>FLOOR(C41*D13,1)</f>
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42">
@@ -966,11 +966,11 @@
       </c>
       <c r="C42" s="8">
         <f>C40-C41</f>
-        <v>7180</v>
+        <v>7182</v>
       </c>
       <c r="D42" s="8">
         <f>FLOOR(C42*D13,1)</f>
-        <v>21540</v>
+        <v>21546</v>
       </c>
     </row>
     <row r="43">
@@ -1006,7 +1006,7 @@
       </c>
       <c r="D46" s="8">
         <f>C46+C42</f>
-        <v>7180</v>
+        <v>7182</v>
       </c>
     </row>
   </sheetData>
@@ -1471,12 +1471,12 @@
         <v>39</v>
       </c>
       <c r="C41" s="8">
-        <f>CEILING(FLOOR(C40*C27,1)*C5,1)</f>
-        <v>20</v>
+        <f>FLOOR(CEILING(FLOOR(D38*C27,1)*C5,1)/D13,1)</f>
+        <v>18</v>
       </c>
       <c r="D41" s="8">
         <f>FLOOR(C41*D13,1)</f>
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42">
@@ -1485,11 +1485,11 @@
       </c>
       <c r="C42" s="8">
         <f>C40-C41</f>
-        <v>9946</v>
+        <v>9948</v>
       </c>
       <c r="D42" s="8">
         <f>FLOOR(C42*D13,1)</f>
-        <v>24865</v>
+        <v>24870</v>
       </c>
     </row>
     <row r="43">
@@ -1525,7 +1525,7 @@
       </c>
       <c r="D46" s="8">
         <f>C46+C42</f>
-        <v>9946</v>
+        <v>9948</v>
       </c>
     </row>
   </sheetData>
@@ -1990,12 +1990,12 @@
         <v>39</v>
       </c>
       <c r="C41" s="8">
-        <f>CEILING(FLOOR(C40*C27,1)*C5,1)</f>
-        <v>20</v>
+        <f>FLOOR(CEILING(FLOOR(D38*C27,1)*C5,1)/D13,1)</f>
+        <v>18</v>
       </c>
       <c r="D41" s="8">
         <f>FLOOR(C41*D13,1)</f>
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42">
@@ -2004,11 +2004,11 @@
       </c>
       <c r="C42" s="8">
         <f>C40-C41</f>
-        <v>9976</v>
+        <v>9978</v>
       </c>
       <c r="D42" s="8">
         <f>FLOOR(C42*D13,1)</f>
-        <v>19952</v>
+        <v>19956</v>
       </c>
     </row>
     <row r="43">
@@ -2044,7 +2044,7 @@
       </c>
       <c r="D46" s="8">
         <f>C46+C42</f>
-        <v>9976</v>
+        <v>9978</v>
       </c>
     </row>
   </sheetData>
@@ -2509,12 +2509,12 @@
         <v>39</v>
       </c>
       <c r="C41" s="8">
-        <f>CEILING(FLOOR(C40*C27,1)*C5,1)</f>
-        <v>1</v>
+        <f>FLOOR(CEILING(FLOOR(D38*C27,1)*C5,1)/D13,1)</f>
+        <v>0</v>
       </c>
       <c r="D41" s="8">
         <f>FLOOR(C41*D13,1)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -2523,11 +2523,11 @@
       </c>
       <c r="C42" s="8">
         <f>C40-C41</f>
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="D42" s="8">
         <f>FLOOR(C42*D13,1)</f>
-        <v>893</v>
+        <v>895</v>
       </c>
     </row>
     <row r="43">
@@ -2563,7 +2563,7 @@
       </c>
       <c r="D46" s="8">
         <f>C46+C42</f>
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="E46" s="9" t="s">
         <v>45</v>
@@ -2978,12 +2978,12 @@
         <v>39</v>
       </c>
       <c r="C39" s="8">
-        <f>CEILING(FLOOR(C38*C25,1)*C5,1)</f>
-        <v>1</v>
+        <f>FLOOR(CEILING(FLOOR(D36*C25,1)*C5,1)/D13,1)</f>
+        <v>0</v>
       </c>
       <c r="D39" s="8">
         <f>FLOOR(C39*D13,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -2992,11 +2992,11 @@
       </c>
       <c r="C40" s="8">
         <f>C38-C39</f>
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="D40" s="8">
         <f>FLOOR(C40*D13,1)</f>
-        <v>1497</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="41">
@@ -3032,7 +3032,7 @@
       </c>
       <c r="D44" s="8">
         <f>C44+C40</f>
-        <v>998</v>
+        <v>999</v>
       </c>
     </row>
   </sheetData>
@@ -3464,7 +3464,7 @@
         <v>39</v>
       </c>
       <c r="C40" s="8">
-        <f>CEILING(FLOOR(C39*C26,1)*C5,1)</f>
+        <f>FLOOR(CEILING(FLOOR(D37*C26,1)*C5,1)/D13,1)</f>
         <v>4</v>
       </c>
       <c r="D40" s="8">

</xml_diff>

<commit_message>
Fix Protocol Liquidation Fee calculation. (#313)
</commit_message>
<xml_diff>
--- a/contracts/red-bank/tests/files/Red Bank - Dynamic LB & CF test cases v1.1.xlsx
+++ b/contracts/red-bank/tests/files/Red Bank - Dynamic LB & CF test cases v1.1.xlsx
@@ -952,12 +952,12 @@
         <v>39</v>
       </c>
       <c r="C41" s="8">
-        <f>CEILING(FLOOR(C40*C27,1)*C5,1)</f>
-        <v>11</v>
+        <f>FLOOR(CEILING(FLOOR(D38*C27,1)*C5,1)/D13,1)</f>
+        <v>9</v>
       </c>
       <c r="D41" s="8">
         <f>FLOOR(C41*D13,1)</f>
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42">
@@ -966,11 +966,11 @@
       </c>
       <c r="C42" s="8">
         <f>C40-C41</f>
-        <v>7180</v>
+        <v>7182</v>
       </c>
       <c r="D42" s="8">
         <f>FLOOR(C42*D13,1)</f>
-        <v>21540</v>
+        <v>21546</v>
       </c>
     </row>
     <row r="43">
@@ -1006,7 +1006,7 @@
       </c>
       <c r="D46" s="8">
         <f>C46+C42</f>
-        <v>7180</v>
+        <v>7182</v>
       </c>
     </row>
   </sheetData>
@@ -1471,12 +1471,12 @@
         <v>39</v>
       </c>
       <c r="C41" s="8">
-        <f>CEILING(FLOOR(C40*C27,1)*C5,1)</f>
-        <v>20</v>
+        <f>FLOOR(CEILING(FLOOR(D38*C27,1)*C5,1)/D13,1)</f>
+        <v>18</v>
       </c>
       <c r="D41" s="8">
         <f>FLOOR(C41*D13,1)</f>
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42">
@@ -1485,11 +1485,11 @@
       </c>
       <c r="C42" s="8">
         <f>C40-C41</f>
-        <v>9946</v>
+        <v>9948</v>
       </c>
       <c r="D42" s="8">
         <f>FLOOR(C42*D13,1)</f>
-        <v>24865</v>
+        <v>24870</v>
       </c>
     </row>
     <row r="43">
@@ -1525,7 +1525,7 @@
       </c>
       <c r="D46" s="8">
         <f>C46+C42</f>
-        <v>9946</v>
+        <v>9948</v>
       </c>
     </row>
   </sheetData>
@@ -1990,12 +1990,12 @@
         <v>39</v>
       </c>
       <c r="C41" s="8">
-        <f>CEILING(FLOOR(C40*C27,1)*C5,1)</f>
-        <v>20</v>
+        <f>FLOOR(CEILING(FLOOR(D38*C27,1)*C5,1)/D13,1)</f>
+        <v>18</v>
       </c>
       <c r="D41" s="8">
         <f>FLOOR(C41*D13,1)</f>
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42">
@@ -2004,11 +2004,11 @@
       </c>
       <c r="C42" s="8">
         <f>C40-C41</f>
-        <v>9976</v>
+        <v>9978</v>
       </c>
       <c r="D42" s="8">
         <f>FLOOR(C42*D13,1)</f>
-        <v>19952</v>
+        <v>19956</v>
       </c>
     </row>
     <row r="43">
@@ -2044,7 +2044,7 @@
       </c>
       <c r="D46" s="8">
         <f>C46+C42</f>
-        <v>9976</v>
+        <v>9978</v>
       </c>
     </row>
   </sheetData>
@@ -2509,12 +2509,12 @@
         <v>39</v>
       </c>
       <c r="C41" s="8">
-        <f>CEILING(FLOOR(C40*C27,1)*C5,1)</f>
-        <v>1</v>
+        <f>FLOOR(CEILING(FLOOR(D38*C27,1)*C5,1)/D13,1)</f>
+        <v>0</v>
       </c>
       <c r="D41" s="8">
         <f>FLOOR(C41*D13,1)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -2523,11 +2523,11 @@
       </c>
       <c r="C42" s="8">
         <f>C40-C41</f>
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="D42" s="8">
         <f>FLOOR(C42*D13,1)</f>
-        <v>893</v>
+        <v>895</v>
       </c>
     </row>
     <row r="43">
@@ -2563,7 +2563,7 @@
       </c>
       <c r="D46" s="8">
         <f>C46+C42</f>
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="E46" s="9" t="s">
         <v>45</v>
@@ -2978,12 +2978,12 @@
         <v>39</v>
       </c>
       <c r="C39" s="8">
-        <f>CEILING(FLOOR(C38*C25,1)*C5,1)</f>
-        <v>1</v>
+        <f>FLOOR(CEILING(FLOOR(D36*C25,1)*C5,1)/D13,1)</f>
+        <v>0</v>
       </c>
       <c r="D39" s="8">
         <f>FLOOR(C39*D13,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -2992,11 +2992,11 @@
       </c>
       <c r="C40" s="8">
         <f>C38-C39</f>
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="D40" s="8">
         <f>FLOOR(C40*D13,1)</f>
-        <v>1497</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="41">
@@ -3032,7 +3032,7 @@
       </c>
       <c r="D44" s="8">
         <f>C44+C40</f>
-        <v>998</v>
+        <v>999</v>
       </c>
     </row>
   </sheetData>
@@ -3464,7 +3464,7 @@
         <v>39</v>
       </c>
       <c r="C40" s="8">
-        <f>CEILING(FLOOR(C39*C26,1)*C5,1)</f>
+        <f>FLOOR(CEILING(FLOOR(D37*C26,1)*C5,1)/D13,1)</f>
         <v>4</v>
       </c>
       <c r="D40" s="8">

</xml_diff>